<commit_message>
favicon ... survey navbar
</commit_message>
<xml_diff>
--- a/kit_urls.xlsx
+++ b/kit_urls.xlsx
@@ -448,120 +448,120 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072025</t>
+          <t>http://localhost:80/12p?name=24082035</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24072025</t>
+          <t>24082035</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072026</t>
+          <t>http://localhost:80/12p?name=24082036</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24072026</t>
+          <t>24082036</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072027</t>
+          <t>http://localhost:80/12p?name=24082037</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24072027</t>
+          <t>24082037</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072028</t>
+          <t>http://localhost:80/12p?name=24082038</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24072028</t>
+          <t>24082038</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072029</t>
+          <t>http://localhost:80/12p?name=24082039</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24072029</t>
+          <t>24082039</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072030</t>
+          <t>http://localhost:80/12p?name=24082040</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>24072030</t>
+          <t>24082040</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072031</t>
+          <t>http://localhost:80/12p?name=24082041</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24072031</t>
+          <t>24082041</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072032</t>
+          <t>http://localhost:80/12p?name=24082042</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24072032</t>
+          <t>24082042</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072033</t>
+          <t>http://localhost:80/12p?name=24082043</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24072033</t>
+          <t>24082043</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24072034</t>
+          <t>http://localhost:80/12p?name=24082044</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24072034</t>
+          <t>24082044</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix database losing connection issue
</commit_message>
<xml_diff>
--- a/kit_urls.xlsx
+++ b/kit_urls.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,120 +448,144 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082035</t>
+          <t>http://request.biomed.hk/12p?name=24082045</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24082035</t>
+          <t>24082045</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082036</t>
+          <t>http://request.biomed.hk/12p?name=24082046</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24082036</t>
+          <t>24082046</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082037</t>
+          <t>http://request.biomed.hk/12p?name=24082047</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24082037</t>
+          <t>24082047</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082038</t>
+          <t>http://request.biomed.hk/12p?name=24082048</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24082038</t>
+          <t>24082048</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082039</t>
+          <t>http://request.biomed.hk/12p?name=24082049</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24082039</t>
+          <t>24082049</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082040</t>
+          <t>http://request.biomed.hk/12p?name=24082050</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>24082040</t>
+          <t>24082050</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082041</t>
+          <t>http://request.biomed.hk/12p?name=24082051</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24082041</t>
+          <t>24082051</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082042</t>
+          <t>http://request.biomed.hk/12p?name=24082052</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24082042</t>
+          <t>24082052</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082043</t>
+          <t>http://request.biomed.hk/12p?name=24082053</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24082043</t>
+          <t>24082053</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>http://localhost:80/12p?name=24082044</t>
+          <t>http://request.biomed.hk/12p?name=24082054</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24082044</t>
+          <t>24082054</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>http://request.biomed.hk/12p?name=24082055</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>24082055</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>http://request.biomed.hk/12p?name=24082056</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>24082056</t>
         </is>
       </c>
     </row>

</xml_diff>